<commit_message>
started PCB, added 3d models for all parts
</commit_message>
<xml_diff>
--- a/Hardware/TalDoor_BOM.xlsx
+++ b/Hardware/TalDoor_BOM.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="21600" windowHeight="11780"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="21600" windowHeight="11780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TalDoor" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -354,9 +354,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -858,10 +858,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1216,11 +1216,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Added connectors, moved notifications to external PCB
</commit_message>
<xml_diff>
--- a/Hardware/TalDoor_BOM.xlsx
+++ b/Hardware/TalDoor_BOM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1200" windowWidth="21600" windowHeight="11780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="21600" windowHeight="11780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TalDoor" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="126">
   <si>
     <t>Component Count:</t>
   </si>
@@ -153,12 +153,6 @@
     <t>Resistor</t>
   </si>
   <si>
-    <t xml:space="preserve">R2, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">R3, R4, </t>
-  </si>
-  <si>
     <t xml:space="preserve">R5, </t>
   </si>
   <si>
@@ -349,6 +343,60 @@
   </si>
   <si>
     <t>S2011EC-09-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q2, Q1, </t>
+  </si>
+  <si>
+    <t>RK7002BM</t>
+  </si>
+  <si>
+    <t>TO_SOT_Packages_SMD:SOT-23</t>
+  </si>
+  <si>
+    <t>Transistor N-MOSFET (general)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R2, R20, R18, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R3, R4, R19, R17, </t>
+  </si>
+  <si>
+    <t>RK7002BMT116CT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J2, </t>
+  </si>
+  <si>
+    <t>Screw_Terminal_01x02</t>
+  </si>
+  <si>
+    <t>Pin_Headers:Pin_Header_Angled_1x02_Pitch2.54mm</t>
+  </si>
+  <si>
+    <t>Generic screw terminal, single row, 01x02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J4, J3, </t>
+  </si>
+  <si>
+    <t>Conn_01x06_Male</t>
+  </si>
+  <si>
+    <t>Connectors_JST:JST_XH_S06B-XH-A_06x2.50mm_Angled</t>
+  </si>
+  <si>
+    <t>Generic connector, single row, 01x06</t>
+  </si>
+  <si>
+    <t>unsure if right angle connectors are even needed</t>
+  </si>
+  <si>
+    <t>455-2236-ND</t>
+  </si>
+  <si>
+    <t>Cables: https://www.amazon.com/uxcell-2-54mm-JST-XH-Adapter-Extension/dp/B014IZWGGI</t>
   </si>
 </sst>
 </file>
@@ -1217,10 +1265,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1237,12 +1285,12 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B2" s="1"/>
     </row>
@@ -1259,7 +1307,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>2</v>
@@ -1271,14 +1319,14 @@
         <v>4</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -1298,7 +1346,7 @@
         <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G5" s="6">
         <v>1.375</v>
@@ -1325,13 +1373,13 @@
         <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G6" s="6">
         <v>1.06E-2</v>
       </c>
       <c r="H6" s="7">
-        <f t="shared" ref="H6:H28" si="0">G6*B6</f>
+        <f t="shared" ref="H6:H31" si="0">G6*B6</f>
         <v>9.5399999999999999E-2</v>
       </c>
     </row>
@@ -1352,7 +1400,7 @@
         <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G7" s="6">
         <v>1.1900000000000001E-2</v>
@@ -1379,7 +1427,7 @@
         <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G8" s="6">
         <v>9.4E-2</v>
@@ -1406,7 +1454,7 @@
         <v>12</v>
       </c>
       <c r="F9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G9" s="6">
         <v>7.4999999999999997E-3</v>
@@ -1433,7 +1481,7 @@
         <v>18</v>
       </c>
       <c r="F10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G10" s="6">
         <v>0.105</v>
@@ -1460,7 +1508,7 @@
         <v>18</v>
       </c>
       <c r="F11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G11" s="6">
         <v>0.33200000000000002</v>
@@ -1484,10 +1532,10 @@
         <v>28</v>
       </c>
       <c r="E12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G12" s="6">
         <v>0.33700000000000002</v>
@@ -1511,10 +1559,10 @@
         <v>28</v>
       </c>
       <c r="E13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G13" s="6">
         <v>0.317</v>
@@ -1538,10 +1586,10 @@
         <v>33</v>
       </c>
       <c r="E14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F14" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G14" s="6">
         <v>4.88</v>
@@ -1553,148 +1601,148 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>115</v>
       </c>
       <c r="B15" s="4">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>35</v>
+        <v>116</v>
       </c>
       <c r="D15" t="s">
-        <v>36</v>
+        <v>117</v>
       </c>
       <c r="E15" t="s">
-        <v>37</v>
-      </c>
-      <c r="F15" t="s">
-        <v>88</v>
-      </c>
-      <c r="G15" s="6">
-        <v>0.14099999999999999</v>
+        <v>118</v>
       </c>
       <c r="H15" s="7">
         <f t="shared" si="0"/>
-        <v>0.14099999999999999</v>
+        <v>0</v>
+      </c>
+      <c r="I15" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>119</v>
       </c>
       <c r="B16" s="4">
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>120</v>
       </c>
       <c r="D16" t="s">
-        <v>40</v>
+        <v>121</v>
       </c>
       <c r="E16" t="s">
-        <v>80</v>
+        <v>122</v>
       </c>
       <c r="F16" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="G16" s="6">
-        <v>0.5</v>
+        <v>0.36799999999999999</v>
       </c>
       <c r="H16" s="7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.73599999999999999</v>
+      </c>
+      <c r="I16" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B17" s="4">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>72</v>
+        <v>35</v>
       </c>
       <c r="D17" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E17" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="F17" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="G17" s="6">
-        <v>8.0000000000000002E-3</v>
+        <v>0.14099999999999999</v>
       </c>
       <c r="H17" s="7">
         <f t="shared" si="0"/>
-        <v>8.0000000000000002E-3</v>
+        <v>0.14099999999999999</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B18" s="4">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" t="s">
+        <v>78</v>
+      </c>
+      <c r="F18" t="s">
+        <v>107</v>
+      </c>
+      <c r="G18" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="H18" s="7">
+        <f t="shared" si="0"/>
         <v>1</v>
-      </c>
-      <c r="C18" t="s">
-        <v>73</v>
-      </c>
-      <c r="D18" t="s">
-        <v>42</v>
-      </c>
-      <c r="E18" t="s">
-        <v>43</v>
-      </c>
-      <c r="F18" t="s">
-        <v>101</v>
-      </c>
-      <c r="G18" s="6">
-        <v>1.6E-2</v>
-      </c>
-      <c r="H18" s="7">
-        <f t="shared" si="0"/>
-        <v>1.6E-2</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>108</v>
       </c>
       <c r="B19" s="4">
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>74</v>
+        <v>109</v>
       </c>
       <c r="D19" t="s">
-        <v>42</v>
+        <v>110</v>
       </c>
       <c r="E19" t="s">
-        <v>43</v>
+        <v>111</v>
       </c>
       <c r="F19" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="G19" s="6">
-        <v>1.2999999999999999E-2</v>
+        <v>0.16</v>
       </c>
       <c r="H19" s="7">
         <f t="shared" si="0"/>
-        <v>2.5999999999999999E-2</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B20" s="4">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D20" t="s">
         <v>42</v>
@@ -1703,25 +1751,25 @@
         <v>43</v>
       </c>
       <c r="F20" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="G20" s="6">
-        <v>1.6E-2</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="H20" s="7">
         <f t="shared" si="0"/>
-        <v>1.6E-2</v>
+        <v>8.0000000000000002E-3</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>47</v>
+        <v>112</v>
       </c>
       <c r="B21" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D21" t="s">
         <v>42</v>
@@ -1730,25 +1778,25 @@
         <v>43</v>
       </c>
       <c r="F21" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="G21" s="6">
-        <v>9.9000000000000008E-3</v>
+        <v>1.6E-2</v>
       </c>
       <c r="H21" s="7">
         <f t="shared" si="0"/>
-        <v>3.9600000000000003E-2</v>
+        <v>4.8000000000000001E-2</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>113</v>
       </c>
       <c r="B22" s="4">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C22" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D22" t="s">
         <v>42</v>
@@ -1757,25 +1805,25 @@
         <v>43</v>
       </c>
       <c r="F22" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="G22" s="6">
-        <v>1.6E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="H22" s="7">
         <f t="shared" si="0"/>
-        <v>9.6000000000000002E-2</v>
+        <v>5.1999999999999998E-2</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B23" s="4">
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D23" t="s">
         <v>42</v>
@@ -1784,7 +1832,7 @@
         <v>43</v>
       </c>
       <c r="F23" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="G23" s="6">
         <v>1.6E-2</v>
@@ -1796,147 +1844,228 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B24" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="D24" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="E24" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="F24" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="G24" s="6">
-        <v>1.2310000000000001</v>
+        <v>9.9000000000000008E-3</v>
       </c>
       <c r="H24" s="7">
         <f t="shared" si="0"/>
-        <v>1.2310000000000001</v>
+        <v>3.9600000000000003E-2</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B25" s="4">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C25" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="D25" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="E25" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="F25" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="G25" s="6">
-        <v>2.7136</v>
+        <v>1.6E-2</v>
       </c>
       <c r="H25" s="7">
         <f t="shared" si="0"/>
-        <v>2.7136</v>
+        <v>9.6000000000000002E-2</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B26" s="4">
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="D26" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="E26" t="s">
-        <v>61</v>
+        <v>43</v>
+      </c>
+      <c r="F26" t="s">
+        <v>104</v>
       </c>
       <c r="G26" s="6">
-        <v>6.63</v>
+        <v>1.6E-2</v>
       </c>
       <c r="H26" s="7">
         <f t="shared" si="0"/>
-        <v>6.63</v>
-      </c>
-      <c r="I26" t="s">
-        <v>59</v>
+        <v>1.6E-2</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="B27" s="4">
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="D27" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="E27" t="s">
-        <v>81</v>
+        <v>51</v>
+      </c>
+      <c r="F27" t="s">
+        <v>105</v>
       </c>
       <c r="G27" s="6">
-        <v>7.29</v>
+        <v>1.2310000000000001</v>
       </c>
       <c r="H27" s="7">
         <f t="shared" si="0"/>
-        <v>7.29</v>
-      </c>
-      <c r="I27" t="s">
-        <v>94</v>
+        <v>1.2310000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="B28" s="4">
         <v>1</v>
       </c>
       <c r="C28" t="s">
+        <v>53</v>
+      </c>
+      <c r="D28" t="s">
+        <v>54</v>
+      </c>
+      <c r="E28" t="s">
+        <v>55</v>
+      </c>
+      <c r="F28" t="s">
+        <v>106</v>
+      </c>
+      <c r="G28" s="6">
+        <v>2.7136</v>
+      </c>
+      <c r="H28" s="7">
+        <f t="shared" si="0"/>
+        <v>2.7136</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="4">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>57</v>
+      </c>
+      <c r="D29" t="s">
+        <v>58</v>
+      </c>
+      <c r="E29" t="s">
+        <v>59</v>
+      </c>
+      <c r="G29" s="6">
+        <v>6.63</v>
+      </c>
+      <c r="H29" s="7">
+        <f t="shared" si="0"/>
+        <v>6.63</v>
+      </c>
+      <c r="I29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" s="4">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>61</v>
+      </c>
+      <c r="D30" t="s">
+        <v>62</v>
+      </c>
+      <c r="E30" t="s">
+        <v>79</v>
+      </c>
+      <c r="G30" s="6">
+        <v>7.29</v>
+      </c>
+      <c r="H30" s="7">
+        <f t="shared" si="0"/>
+        <v>7.29</v>
+      </c>
+      <c r="I30" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31" s="4">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s">
+        <v>64</v>
+      </c>
+      <c r="D31" t="s">
+        <v>65</v>
+      </c>
+      <c r="E31" t="s">
         <v>66</v>
       </c>
-      <c r="D28" t="s">
-        <v>67</v>
-      </c>
-      <c r="E28" t="s">
-        <v>68</v>
-      </c>
-      <c r="F28" t="s">
-        <v>84</v>
-      </c>
-      <c r="G28" s="6">
+      <c r="F31" t="s">
+        <v>82</v>
+      </c>
+      <c r="G31" s="6">
         <v>0.25</v>
       </c>
-      <c r="H28" s="7">
+      <c r="H31" s="7">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="G30" s="8">
-        <f>SUM(H5:H28)</f>
-        <v>28.441899999999997</v>
-      </c>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C33" s="5"/>
+    <row r="33" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="G33" s="8">
+        <f>SUM(H5:H31)</f>
+        <v>29.555899999999998</v>
+      </c>
+    </row>
+    <row r="36" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C36" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Solution to 1 wire LED nitification issue. See LED_NotificationModel.txt
</commit_message>
<xml_diff>
--- a/Hardware/TalDoor_BOM.xlsx
+++ b/Hardware/TalDoor_BOM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1800" windowWidth="21600" windowHeight="11780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2400" windowWidth="21600" windowHeight="11780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TalDoor" sheetId="1" r:id="rId1"/>
@@ -180,15 +180,6 @@
     <t xml:space="preserve">U2, </t>
   </si>
   <si>
-    <t>ENC28J60-C/SS</t>
-  </si>
-  <si>
-    <t>Housings_SSOP:SSOP-28_5.3x10.2mm_Pitch0.65mm</t>
-  </si>
-  <si>
-    <t>ENC28J60 Single Chip Ethernet Interface, SSOP-28</t>
-  </si>
-  <si>
     <t xml:space="preserve">U3, </t>
   </si>
   <si>
@@ -339,9 +330,6 @@
     <t>296-34806-1-ND</t>
   </si>
   <si>
-    <t>ENC28J60/SS-ND</t>
-  </si>
-  <si>
     <t>S2011EC-09-ND</t>
   </si>
   <si>
@@ -397,6 +385,18 @@
   </si>
   <si>
     <t>Cables: https://www.amazon.com/uxcell-2-54mm-JST-XH-Adapter-Extension/dp/B014IZWGGI</t>
+  </si>
+  <si>
+    <t>ENC28J60-I/SO-ND</t>
+  </si>
+  <si>
+    <t>ENC28J60-I/SO</t>
+  </si>
+  <si>
+    <t>ENC28J60 Single Chip Ethernet Interface, SOIC-28</t>
+  </si>
+  <si>
+    <t>Housings_SOIC:SOIC-28W_7.5x17.9mm_Pitch1.27mm</t>
   </si>
 </sst>
 </file>
@@ -1267,8 +1267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1285,12 +1285,12 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B2" s="1"/>
     </row>
@@ -1307,7 +1307,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>2</v>
@@ -1319,14 +1319,14 @@
         <v>4</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -1346,7 +1346,7 @@
         <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G5" s="6">
         <v>1.375</v>
@@ -1373,7 +1373,7 @@
         <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G6" s="6">
         <v>1.06E-2</v>
@@ -1400,7 +1400,7 @@
         <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G7" s="6">
         <v>1.1900000000000001E-2</v>
@@ -1427,7 +1427,7 @@
         <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G8" s="6">
         <v>9.4E-2</v>
@@ -1454,7 +1454,7 @@
         <v>12</v>
       </c>
       <c r="F9" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G9" s="6">
         <v>7.4999999999999997E-3</v>
@@ -1481,7 +1481,7 @@
         <v>18</v>
       </c>
       <c r="F10" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G10" s="6">
         <v>0.105</v>
@@ -1508,7 +1508,7 @@
         <v>18</v>
       </c>
       <c r="F11" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G11" s="6">
         <v>0.33200000000000002</v>
@@ -1532,10 +1532,10 @@
         <v>28</v>
       </c>
       <c r="E12" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F12" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G12" s="6">
         <v>0.33700000000000002</v>
@@ -1559,10 +1559,10 @@
         <v>28</v>
       </c>
       <c r="E13" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F13" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G13" s="6">
         <v>0.317</v>
@@ -1586,10 +1586,10 @@
         <v>33</v>
       </c>
       <c r="E14" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F14" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G14" s="6">
         <v>4.88</v>
@@ -1601,46 +1601,46 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B15" s="4">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D15" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E15" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="H15" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B16" s="4">
         <v>2</v>
       </c>
       <c r="C16" t="s">
+        <v>116</v>
+      </c>
+      <c r="D16" t="s">
+        <v>117</v>
+      </c>
+      <c r="E16" t="s">
+        <v>118</v>
+      </c>
+      <c r="F16" t="s">
         <v>120</v>
-      </c>
-      <c r="D16" t="s">
-        <v>121</v>
-      </c>
-      <c r="E16" t="s">
-        <v>122</v>
-      </c>
-      <c r="F16" t="s">
-        <v>124</v>
       </c>
       <c r="G16" s="6">
         <v>0.36799999999999999</v>
@@ -1650,7 +1650,7 @@
         <v>0.73599999999999999</v>
       </c>
       <c r="I16" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
@@ -1670,7 +1670,7 @@
         <v>37</v>
       </c>
       <c r="F17" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G17" s="6">
         <v>0.14099999999999999</v>
@@ -1694,10 +1694,10 @@
         <v>40</v>
       </c>
       <c r="E18" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F18" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G18" s="6">
         <v>0.5</v>
@@ -1709,22 +1709,22 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B19" s="4">
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D19" t="s">
+        <v>106</v>
+      </c>
+      <c r="E19" t="s">
+        <v>107</v>
+      </c>
+      <c r="F19" t="s">
         <v>110</v>
-      </c>
-      <c r="E19" t="s">
-        <v>111</v>
-      </c>
-      <c r="F19" t="s">
-        <v>114</v>
       </c>
       <c r="G19" s="6">
         <v>0.16</v>
@@ -1742,7 +1742,7 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D20" t="s">
         <v>42</v>
@@ -1751,7 +1751,7 @@
         <v>43</v>
       </c>
       <c r="F20" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G20" s="6">
         <v>8.0000000000000002E-3</v>
@@ -1763,13 +1763,13 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B21" s="4">
         <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D21" t="s">
         <v>42</v>
@@ -1778,7 +1778,7 @@
         <v>43</v>
       </c>
       <c r="F21" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="G21" s="6">
         <v>1.6E-2</v>
@@ -1790,13 +1790,13 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B22" s="4">
         <v>4</v>
       </c>
       <c r="C22" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D22" t="s">
         <v>42</v>
@@ -1805,7 +1805,7 @@
         <v>43</v>
       </c>
       <c r="F22" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G22" s="6">
         <v>1.2999999999999999E-2</v>
@@ -1823,7 +1823,7 @@
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D23" t="s">
         <v>42</v>
@@ -1832,7 +1832,7 @@
         <v>43</v>
       </c>
       <c r="F23" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G23" s="6">
         <v>1.6E-2</v>
@@ -1850,7 +1850,7 @@
         <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D24" t="s">
         <v>42</v>
@@ -1859,7 +1859,7 @@
         <v>43</v>
       </c>
       <c r="F24" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G24" s="6">
         <v>9.9000000000000008E-3</v>
@@ -1877,7 +1877,7 @@
         <v>6</v>
       </c>
       <c r="C25" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D25" t="s">
         <v>42</v>
@@ -1886,7 +1886,7 @@
         <v>43</v>
       </c>
       <c r="F25" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G25" s="6">
         <v>1.6E-2</v>
@@ -1904,7 +1904,7 @@
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D26" t="s">
         <v>42</v>
@@ -1913,7 +1913,7 @@
         <v>43</v>
       </c>
       <c r="F26" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G26" s="6">
         <v>1.6E-2</v>
@@ -1940,7 +1940,7 @@
         <v>51</v>
       </c>
       <c r="F27" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G27" s="6">
         <v>1.2310000000000001</v>
@@ -1958,40 +1958,40 @@
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>53</v>
+        <v>123</v>
       </c>
       <c r="D28" t="s">
-        <v>54</v>
+        <v>125</v>
       </c>
       <c r="E28" t="s">
-        <v>55</v>
+        <v>124</v>
       </c>
       <c r="F28" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="G28" s="6">
-        <v>2.7136</v>
+        <v>2.7559999999999998</v>
       </c>
       <c r="H28" s="7">
         <f t="shared" si="0"/>
-        <v>2.7136</v>
+        <v>2.7559999999999998</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B29" s="4">
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D29" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E29" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G29" s="6">
         <v>6.63</v>
@@ -2001,24 +2001,24 @@
         <v>6.63</v>
       </c>
       <c r="I29" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B30" s="4">
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D30" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E30" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G30" s="6">
         <v>7.29</v>
@@ -2028,27 +2028,27 @@
         <v>7.29</v>
       </c>
       <c r="I30" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B31" s="4">
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D31" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E31" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F31" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G31" s="6">
         <v>0.25</v>
@@ -2061,7 +2061,7 @@
     <row r="33" spans="3:7" x14ac:dyDescent="0.35">
       <c r="G33" s="8">
         <f>SUM(H5:H31)</f>
-        <v>29.555899999999998</v>
+        <v>29.598299999999998</v>
       </c>
     </row>
     <row r="36" spans="3:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updated schematic with N/Pmos LED format for single IO drive. Updated BOM
</commit_message>
<xml_diff>
--- a/Hardware/TalDoor_BOM.xlsx
+++ b/Hardware/TalDoor_BOM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2400" windowWidth="21600" windowHeight="11780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3000" windowWidth="21600" windowHeight="11780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TalDoor" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="133">
   <si>
     <t>Component Count:</t>
   </si>
@@ -99,18 +99,12 @@
     <t>Capacitors_THT:CP_Radial_D10.0mm_P5.00mm</t>
   </si>
   <si>
-    <t xml:space="preserve">D2, D1, D3, </t>
-  </si>
-  <si>
     <t>G_LED</t>
   </si>
   <si>
     <t>LEDs:LED_0603</t>
   </si>
   <si>
-    <t xml:space="preserve">D4, D5, D6, </t>
-  </si>
-  <si>
     <t>R_LED</t>
   </si>
   <si>
@@ -159,12 +153,6 @@
     <t xml:space="preserve">R9, R8, R7, R6, </t>
   </si>
   <si>
-    <t xml:space="preserve">R13, R10, R11, R12, R14, R15, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">R16, </t>
-  </si>
-  <si>
     <t xml:space="preserve">U1, </t>
   </si>
   <si>
@@ -216,9 +204,6 @@
     <t xml:space="preserve">TalDoor PCB </t>
   </si>
   <si>
-    <t>Generated: 1/1/2018  6:17:19 PM</t>
-  </si>
-  <si>
     <t>QTY</t>
   </si>
   <si>
@@ -333,9 +318,6 @@
     <t>S2011EC-09-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">Q2, Q1, </t>
-  </si>
-  <si>
     <t>RK7002BM</t>
   </si>
   <si>
@@ -345,12 +327,6 @@
     <t>Transistor N-MOSFET (general)</t>
   </si>
   <si>
-    <t xml:space="preserve">R2, R20, R18, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">R3, R4, R19, R17, </t>
-  </si>
-  <si>
     <t>RK7002BMT116CT-ND</t>
   </si>
   <si>
@@ -397,6 +373,51 @@
   </si>
   <si>
     <t>Housings_SOIC:SOIC-28W_7.5x17.9mm_Pitch1.27mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R19, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R14, R10, R11, R12, R15, R16, R13, R17, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R3, R4, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R2, R18, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q2, </t>
+  </si>
+  <si>
+    <t>BSS223PWH6327XTSA1</t>
+  </si>
+  <si>
+    <t>TO_SOT_Packages_SMD:SOT-323_SC-70</t>
+  </si>
+  <si>
+    <t>P-MOSFET with substrate diode BSS223PWH6327XTSA1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q1, </t>
+  </si>
+  <si>
+    <t>Pmos</t>
+  </si>
+  <si>
+    <t>Nmos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D2, D1, D3, D4, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">D5, D6, D7, D8, </t>
+  </si>
+  <si>
+    <t>BSS223PWH6327XTSA1CT-ND</t>
+  </si>
+  <si>
+    <t>Generated: 1/4/2018  3:25:19 PM</t>
   </si>
 </sst>
 </file>
@@ -892,7 +913,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -910,6 +931,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1265,41 +1289,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.08984375" customWidth="1"/>
+    <col min="1" max="1" width="33.36328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.6328125" customWidth="1"/>
     <col min="5" max="5" width="43.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.6328125" customWidth="1"/>
+    <col min="6" max="6" width="25.54296875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.26953125" customWidth="1"/>
     <col min="9" max="9" width="48.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>132</v>
       </c>
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B3">
-        <v>48</v>
+        <f>SUM(B5:B42)</f>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1307,7 +1332,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>2</v>
@@ -1319,14 +1344,14 @@
         <v>4</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -1346,7 +1371,7 @@
         <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="G5" s="6">
         <v>1.375</v>
@@ -1373,13 +1398,13 @@
         <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="G6" s="6">
         <v>1.06E-2</v>
       </c>
       <c r="H6" s="7">
-        <f t="shared" ref="H6:H31" si="0">G6*B6</f>
+        <f t="shared" ref="H6:H32" si="0">G6*B6</f>
         <v>9.5399999999999999E-2</v>
       </c>
     </row>
@@ -1400,7 +1425,7 @@
         <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="G7" s="6">
         <v>1.1900000000000001E-2</v>
@@ -1427,7 +1452,7 @@
         <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="G8" s="6">
         <v>9.4E-2</v>
@@ -1454,7 +1479,7 @@
         <v>12</v>
       </c>
       <c r="F9" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="G9" s="6">
         <v>7.4999999999999997E-3</v>
@@ -1481,7 +1506,7 @@
         <v>18</v>
       </c>
       <c r="F10" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="G10" s="6">
         <v>0.105</v>
@@ -1508,7 +1533,7 @@
         <v>18</v>
       </c>
       <c r="F11" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="G11" s="6">
         <v>0.33200000000000002</v>
@@ -1520,76 +1545,76 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>129</v>
+      </c>
+      <c r="B12" s="4">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="4">
-        <v>3</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>27</v>
       </c>
-      <c r="D12" t="s">
-        <v>28</v>
-      </c>
       <c r="E12" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F12" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="G12" s="6">
         <v>0.33700000000000002</v>
       </c>
       <c r="H12" s="7">
         <f t="shared" si="0"/>
-        <v>1.0110000000000001</v>
+        <v>1.3480000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>130</v>
       </c>
       <c r="B13" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E13" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="F13" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="G13" s="6">
         <v>0.317</v>
       </c>
       <c r="H13" s="7">
         <f t="shared" si="0"/>
-        <v>0.95100000000000007</v>
+        <v>1.268</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B14" s="4">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E14" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F14" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="G14" s="6">
         <v>4.88</v>
@@ -1601,46 +1626,49 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B15" s="4">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="D15" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="E15" t="s">
-        <v>114</v>
+        <v>106</v>
+      </c>
+      <c r="G15" s="6">
+        <v>0</v>
       </c>
       <c r="H15" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="B16" s="4">
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="D16" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="E16" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="F16" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="G16" s="6">
         <v>0.36799999999999999</v>
@@ -1650,27 +1678,27 @@
         <v>0.73599999999999999</v>
       </c>
       <c r="I16" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B17" s="4">
         <v>1</v>
       </c>
       <c r="C17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" t="s">
         <v>35</v>
       </c>
-      <c r="D17" t="s">
-        <v>36</v>
-      </c>
-      <c r="E17" t="s">
-        <v>37</v>
-      </c>
       <c r="F17" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G17" s="6">
         <v>0.14099999999999999</v>
@@ -1682,22 +1710,22 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B18" s="4">
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E18" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F18" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="G18" s="6">
         <v>0.5</v>
@@ -1709,363 +1737,396 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>104</v>
+        <v>126</v>
       </c>
       <c r="B19" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D19" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E19" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="F19" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="G19" s="6">
         <v>0.16</v>
       </c>
       <c r="H19" s="7">
         <f t="shared" si="0"/>
-        <v>0.32</v>
+        <v>0.16</v>
+      </c>
+      <c r="I19" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>122</v>
       </c>
       <c r="B20" s="4">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>67</v>
+        <v>123</v>
       </c>
       <c r="D20" t="s">
-        <v>42</v>
+        <v>124</v>
       </c>
       <c r="E20" t="s">
-        <v>43</v>
+        <v>125</v>
       </c>
       <c r="F20" t="s">
-        <v>95</v>
+        <v>131</v>
       </c>
       <c r="G20" s="6">
-        <v>8.0000000000000002E-3</v>
+        <v>0.30299999999999999</v>
       </c>
       <c r="H20" s="7">
         <f t="shared" si="0"/>
-        <v>8.0000000000000002E-3</v>
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="I20" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>108</v>
+        <v>39</v>
       </c>
       <c r="B21" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D21" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E21" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F21" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="G21" s="6">
-        <v>1.6E-2</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="H21" s="7">
         <f t="shared" si="0"/>
-        <v>4.8000000000000001E-2</v>
+        <v>8.0000000000000002E-3</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="B22" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D22" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E22" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F22" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="G22" s="6">
-        <v>1.2999999999999999E-2</v>
+        <v>1.6E-2</v>
       </c>
       <c r="H22" s="7">
         <f t="shared" si="0"/>
-        <v>5.1999999999999998E-2</v>
+        <v>3.2000000000000001E-2</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>120</v>
       </c>
       <c r="B23" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D23" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E23" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F23" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="G23" s="6">
-        <v>1.6E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="H23" s="7">
         <f t="shared" si="0"/>
-        <v>1.6E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B24" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D24" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E24" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F24" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="G24" s="6">
-        <v>9.9000000000000008E-3</v>
+        <v>1.6E-2</v>
       </c>
       <c r="H24" s="7">
         <f t="shared" si="0"/>
-        <v>3.9600000000000003E-2</v>
+        <v>1.6E-2</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B25" s="4">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C25" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D25" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E25" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F25" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="G25" s="6">
-        <v>1.6E-2</v>
+        <v>9.9000000000000008E-3</v>
       </c>
       <c r="H25" s="7">
         <f t="shared" si="0"/>
-        <v>9.6000000000000002E-2</v>
+        <v>3.9600000000000003E-2</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>47</v>
+        <v>119</v>
       </c>
       <c r="B26" s="4">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C26" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D26" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E26" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F26" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="G26" s="6">
         <v>1.6E-2</v>
       </c>
       <c r="H26" s="7">
         <f t="shared" si="0"/>
-        <v>1.6E-2</v>
+        <v>0.128</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>48</v>
+        <v>118</v>
       </c>
       <c r="B27" s="4">
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D27" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E27" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="F27" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G27" s="6">
-        <v>1.2310000000000001</v>
+        <v>1.6E-2</v>
       </c>
       <c r="H27" s="7">
         <f t="shared" si="0"/>
-        <v>1.2310000000000001</v>
+        <v>1.6E-2</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B28" s="4">
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>123</v>
+        <v>45</v>
       </c>
       <c r="D28" t="s">
-        <v>125</v>
+        <v>46</v>
       </c>
       <c r="E28" t="s">
-        <v>124</v>
+        <v>47</v>
       </c>
       <c r="F28" t="s">
-        <v>122</v>
+        <v>97</v>
       </c>
       <c r="G28" s="6">
-        <v>2.7559999999999998</v>
+        <v>1.2310000000000001</v>
       </c>
       <c r="H28" s="7">
         <f t="shared" si="0"/>
-        <v>2.7559999999999998</v>
+        <v>1.2310000000000001</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B29" s="4">
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>54</v>
+        <v>115</v>
       </c>
       <c r="D29" t="s">
-        <v>55</v>
+        <v>117</v>
       </c>
       <c r="E29" t="s">
-        <v>56</v>
+        <v>116</v>
+      </c>
+      <c r="F29" t="s">
+        <v>114</v>
       </c>
       <c r="G29" s="6">
-        <v>6.63</v>
+        <v>2.7559999999999998</v>
       </c>
       <c r="H29" s="7">
         <f t="shared" si="0"/>
-        <v>6.63</v>
-      </c>
-      <c r="I29" t="s">
-        <v>54</v>
+        <v>2.7559999999999998</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B30" s="4">
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D30" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E30" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="G30" s="6">
-        <v>7.29</v>
+        <v>6.63</v>
       </c>
       <c r="H30" s="7">
         <f t="shared" si="0"/>
-        <v>7.29</v>
+        <v>6.63</v>
       </c>
       <c r="I30" t="s">
-        <v>89</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B31" s="4">
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D31" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E31" t="s">
-        <v>63</v>
-      </c>
-      <c r="F31" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="G31" s="6">
+        <v>7.29</v>
+      </c>
+      <c r="H31" s="7">
+        <f t="shared" si="0"/>
+        <v>7.29</v>
+      </c>
+      <c r="I31" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32" s="4">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>57</v>
+      </c>
+      <c r="D32" t="s">
+        <v>58</v>
+      </c>
+      <c r="E32" t="s">
+        <v>59</v>
+      </c>
+      <c r="F32" t="s">
+        <v>74</v>
+      </c>
+      <c r="G32" s="6">
         <v>0.25</v>
       </c>
-      <c r="H31" s="7">
+      <c r="H32" s="7">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
     </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="G33" s="8">
-        <f>SUM(H5:H31)</f>
-        <v>29.598299999999998</v>
-      </c>
-    </row>
-    <row r="36" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C36" s="5"/>
+    <row r="34" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="G34" s="8">
+        <f>SUM(H5:H32)</f>
+        <v>30.385299999999997</v>
+      </c>
+    </row>
+    <row r="37" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C37" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Completed Mainboard PCB, needs Vgroove/Mousebite connection between two. Also check motor driver
</commit_message>
<xml_diff>
--- a/Hardware/TalDoor_BOM.xlsx
+++ b/Hardware/TalDoor_BOM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3000" windowWidth="21600" windowHeight="11780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3600" windowWidth="21600" windowHeight="11780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TalDoor" sheetId="1" r:id="rId1"/>
@@ -129,15 +129,6 @@
     <t>Ferrite bead</t>
   </si>
   <si>
-    <t xml:space="preserve">P1, P2, </t>
-  </si>
-  <si>
-    <t>Conn_02x18_Odd_Even</t>
-  </si>
-  <si>
-    <t>Pin_Headers:Pin_Header_Straight_2x18_Pitch2.54mm</t>
-  </si>
-  <si>
     <t xml:space="preserve">R1, </t>
   </si>
   <si>
@@ -315,9 +306,6 @@
     <t>296-34806-1-ND</t>
   </si>
   <si>
-    <t>S2011EC-09-ND</t>
-  </si>
-  <si>
     <t>RK7002BM</t>
   </si>
   <si>
@@ -418,6 +406,18 @@
   </si>
   <si>
     <t>Generated: 1/4/2018  3:25:19 PM</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>PocketBeagle</t>
+  </si>
+  <si>
+    <t>Bespoke Male Pin Headers</t>
+  </si>
+  <si>
+    <t>TalDoor_Footprints:PocketBeagle_TalDoor</t>
   </si>
 </sst>
 </file>
@@ -1291,8 +1291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1309,12 +1309,12 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B2" s="1"/>
     </row>
@@ -1324,7 +1324,7 @@
       </c>
       <c r="B3">
         <f>SUM(B5:B42)</f>
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1332,7 +1332,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>2</v>
@@ -1344,14 +1344,14 @@
         <v>4</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -1371,7 +1371,7 @@
         <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G5" s="6">
         <v>1.375</v>
@@ -1398,7 +1398,7 @@
         <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G6" s="6">
         <v>1.06E-2</v>
@@ -1425,7 +1425,7 @@
         <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G7" s="6">
         <v>1.1900000000000001E-2</v>
@@ -1452,7 +1452,7 @@
         <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G8" s="6">
         <v>9.4E-2</v>
@@ -1479,7 +1479,7 @@
         <v>12</v>
       </c>
       <c r="F9" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G9" s="6">
         <v>7.4999999999999997E-3</v>
@@ -1506,7 +1506,7 @@
         <v>18</v>
       </c>
       <c r="F10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G10" s="6">
         <v>0.105</v>
@@ -1533,7 +1533,7 @@
         <v>18</v>
       </c>
       <c r="F11" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G11" s="6">
         <v>0.33200000000000002</v>
@@ -1545,7 +1545,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B12" s="4">
         <v>4</v>
@@ -1557,10 +1557,10 @@
         <v>27</v>
       </c>
       <c r="E12" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F12" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G12" s="6">
         <v>0.33700000000000002</v>
@@ -1572,7 +1572,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B13" s="4">
         <v>4</v>
@@ -1584,10 +1584,10 @@
         <v>27</v>
       </c>
       <c r="E13" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F13" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G13" s="6">
         <v>0.317</v>
@@ -1611,10 +1611,10 @@
         <v>31</v>
       </c>
       <c r="E14" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F14" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G14" s="6">
         <v>4.88</v>
@@ -1626,19 +1626,19 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B15" s="4">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D15" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E15" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G15" s="6">
         <v>0</v>
@@ -1648,27 +1648,27 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B16" s="4">
         <v>2</v>
       </c>
       <c r="C16" t="s">
+        <v>104</v>
+      </c>
+      <c r="D16" t="s">
+        <v>105</v>
+      </c>
+      <c r="E16" t="s">
+        <v>106</v>
+      </c>
+      <c r="F16" t="s">
         <v>108</v>
-      </c>
-      <c r="D16" t="s">
-        <v>109</v>
-      </c>
-      <c r="E16" t="s">
-        <v>110</v>
-      </c>
-      <c r="F16" t="s">
-        <v>112</v>
       </c>
       <c r="G16" s="6">
         <v>0.36799999999999999</v>
@@ -1678,7 +1678,7 @@
         <v>0.73599999999999999</v>
       </c>
       <c r="I16" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
@@ -1698,7 +1698,7 @@
         <v>35</v>
       </c>
       <c r="F17" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G17" s="6">
         <v>0.14099999999999999</v>
@@ -1710,49 +1710,47 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>129</v>
       </c>
       <c r="B18" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>37</v>
+        <v>130</v>
       </c>
       <c r="D18" t="s">
-        <v>38</v>
+        <v>132</v>
       </c>
       <c r="E18" t="s">
-        <v>70</v>
-      </c>
-      <c r="F18" t="s">
-        <v>98</v>
-      </c>
-      <c r="G18" s="6">
-        <v>0.5</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="G18" s="6"/>
       <c r="H18" s="7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="I18" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B19" s="4">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D19" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E19" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F19" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G19" s="6">
         <v>0.16</v>
@@ -1762,27 +1760,27 @@
         <v>0.16</v>
       </c>
       <c r="I19" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B20" s="4">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D20" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E20" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="F20" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="G20" s="6">
         <v>0.30299999999999999</v>
@@ -1792,27 +1790,27 @@
         <v>0.30299999999999999</v>
       </c>
       <c r="I20" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B21" s="4">
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D21" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E21" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F21" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G21" s="6">
         <v>8.0000000000000002E-3</v>
@@ -1824,22 +1822,22 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B22" s="4">
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D22" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E22" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F22" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="G22" s="6">
         <v>1.6E-2</v>
@@ -1851,22 +1849,22 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B23" s="4">
         <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D23" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E23" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F23" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G23" s="6">
         <v>1.2999999999999999E-2</v>
@@ -1878,22 +1876,22 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B24" s="4">
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D24" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E24" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F24" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="G24" s="6">
         <v>1.6E-2</v>
@@ -1905,22 +1903,22 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B25" s="4">
         <v>4</v>
       </c>
       <c r="C25" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D25" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E25" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F25" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G25" s="6">
         <v>9.9000000000000008E-3</v>
@@ -1932,22 +1930,22 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B26" s="4">
         <v>8</v>
       </c>
       <c r="C26" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D26" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E26" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F26" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G26" s="6">
         <v>1.6E-2</v>
@@ -1959,22 +1957,22 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B27" s="4">
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D27" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E27" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F27" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G27" s="6">
         <v>1.6E-2</v>
@@ -1986,22 +1984,22 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B28" s="4">
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D28" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E28" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F28" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G28" s="6">
         <v>1.2310000000000001</v>
@@ -2013,22 +2011,22 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B29" s="4">
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D29" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E29" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="F29" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="G29" s="6">
         <v>2.7559999999999998</v>
@@ -2040,19 +2038,19 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B30" s="4">
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D30" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E30" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G30" s="6">
         <v>6.63</v>
@@ -2062,24 +2060,24 @@
         <v>6.63</v>
       </c>
       <c r="I30" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B31" s="4">
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D31" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E31" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G31" s="6">
         <v>7.29</v>
@@ -2089,27 +2087,27 @@
         <v>7.29</v>
       </c>
       <c r="I31" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B32" s="4">
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D32" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E32" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F32" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G32" s="6">
         <v>0.25</v>
@@ -2122,7 +2120,7 @@
     <row r="34" spans="3:7" x14ac:dyDescent="0.35">
       <c r="G34" s="8">
         <f>SUM(H5:H32)</f>
-        <v>30.385299999999997</v>
+        <v>29.385300000000001</v>
       </c>
     </row>
     <row r="37" spans="3:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Added 5v motor control. Updated schematic, images, BOM, PCB layout
</commit_message>
<xml_diff>
--- a/Hardware/TalDoor_BOM.xlsx
+++ b/Hardware/TalDoor_BOM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3600" windowWidth="21600" windowHeight="11780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="4200" windowWidth="21600" windowHeight="11780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TalDoor" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="141">
   <si>
     <t>Component Count:</t>
   </si>
@@ -405,9 +405,6 @@
     <t>BSS223PWH6327XTSA1CT-ND</t>
   </si>
   <si>
-    <t>Generated: 1/4/2018  3:25:19 PM</t>
-  </si>
-  <si>
     <t>P1</t>
   </si>
   <si>
@@ -418,6 +415,33 @@
   </si>
   <si>
     <t>TalDoor_Footprints:PocketBeagle_TalDoor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C18, C19, C17, </t>
+  </si>
+  <si>
+    <t>1uF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U5, </t>
+  </si>
+  <si>
+    <t>CAT3200-5</t>
+  </si>
+  <si>
+    <t>TO_SOT_Packages_SMD:SOT-23-6</t>
+  </si>
+  <si>
+    <t>Charge Pump Switching Regulator IC Positive Fixed 5V 1 Output 100mA SOT-23-6</t>
+  </si>
+  <si>
+    <t>CAT3200TDI-GT3OSCT-ND</t>
+  </si>
+  <si>
+    <t>311-3484-1-ND</t>
+  </si>
+  <si>
+    <t>Generated: 1/6/2018  3:56:19 PM</t>
   </si>
 </sst>
 </file>
@@ -1289,10 +1313,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1314,7 +1338,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="B2" s="1"/>
     </row>
@@ -1323,8 +1347,8 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <f>SUM(B5:B42)</f>
-        <v>57</v>
+        <f>SUM(B5:B44)</f>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1404,7 +1428,7 @@
         <v>1.06E-2</v>
       </c>
       <c r="H6" s="7">
-        <f t="shared" ref="H6:H32" si="0">G6*B6</f>
+        <f t="shared" ref="H6:H34" si="0">G6*B6</f>
         <v>9.5399999999999999E-2</v>
       </c>
     </row>
@@ -1545,290 +1569,290 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="B12" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>133</v>
       </c>
       <c r="D12" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="F12" t="s">
-        <v>78</v>
+        <v>139</v>
       </c>
       <c r="G12" s="6">
-        <v>0.33700000000000002</v>
+        <v>5.8200000000000002E-2</v>
       </c>
       <c r="H12" s="7">
         <f t="shared" si="0"/>
-        <v>1.3480000000000001</v>
+        <v>0.17460000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B13" s="4">
         <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D13" t="s">
         <v>27</v>
       </c>
       <c r="E13" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G13" s="6">
-        <v>0.317</v>
+        <v>0.33700000000000002</v>
       </c>
       <c r="H13" s="7">
         <f t="shared" si="0"/>
-        <v>1.268</v>
+        <v>1.3480000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>126</v>
       </c>
       <c r="B14" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D14" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E14" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="F14" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G14" s="6">
-        <v>4.88</v>
+        <v>0.317</v>
       </c>
       <c r="H14" s="7">
         <f t="shared" si="0"/>
-        <v>4.88</v>
+        <v>1.268</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>99</v>
+        <v>29</v>
       </c>
       <c r="B15" s="4">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>101</v>
+        <v>31</v>
       </c>
       <c r="E15" t="s">
-        <v>102</v>
+        <v>66</v>
+      </c>
+      <c r="F15" t="s">
+        <v>83</v>
       </c>
       <c r="G15" s="6">
-        <v>0</v>
+        <v>4.88</v>
       </c>
       <c r="H15" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I15" t="s">
-        <v>107</v>
+        <v>4.88</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B16" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D16" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E16" t="s">
-        <v>106</v>
-      </c>
-      <c r="F16" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="G16" s="6">
-        <v>0.36799999999999999</v>
+        <v>0</v>
       </c>
       <c r="H16" s="7">
         <f t="shared" si="0"/>
-        <v>0.73599999999999999</v>
+        <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>103</v>
       </c>
       <c r="B17" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>104</v>
       </c>
       <c r="D17" t="s">
-        <v>34</v>
+        <v>105</v>
       </c>
       <c r="E17" t="s">
-        <v>35</v>
+        <v>106</v>
       </c>
       <c r="F17" t="s">
-        <v>75</v>
+        <v>108</v>
       </c>
       <c r="G17" s="6">
-        <v>0.14099999999999999</v>
+        <v>0.36799999999999999</v>
       </c>
       <c r="H17" s="7">
         <f t="shared" si="0"/>
-        <v>0.14099999999999999</v>
+        <v>0.73599999999999999</v>
+      </c>
+      <c r="I17" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>129</v>
+        <v>32</v>
       </c>
       <c r="B18" s="4">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>130</v>
+        <v>33</v>
       </c>
       <c r="D18" t="s">
-        <v>132</v>
+        <v>34</v>
       </c>
       <c r="E18" t="s">
-        <v>67</v>
-      </c>
-      <c r="G18" s="6"/>
+        <v>35</v>
+      </c>
+      <c r="F18" t="s">
+        <v>75</v>
+      </c>
+      <c r="G18" s="6">
+        <v>0.14099999999999999</v>
+      </c>
       <c r="H18" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I18" t="s">
-        <v>131</v>
+        <v>0.14099999999999999</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="B19" s="4">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>95</v>
+        <v>129</v>
       </c>
       <c r="D19" t="s">
-        <v>96</v>
+        <v>131</v>
       </c>
       <c r="E19" t="s">
-        <v>97</v>
-      </c>
-      <c r="F19" t="s">
-        <v>98</v>
-      </c>
-      <c r="G19" s="6">
-        <v>0.16</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="G19" s="6"/>
       <c r="H19" s="7">
         <f t="shared" si="0"/>
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="I19" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B20" s="4">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>119</v>
+        <v>95</v>
       </c>
       <c r="D20" t="s">
-        <v>120</v>
+        <v>96</v>
       </c>
       <c r="E20" t="s">
-        <v>121</v>
+        <v>97</v>
       </c>
       <c r="F20" t="s">
-        <v>127</v>
+        <v>98</v>
       </c>
       <c r="G20" s="6">
-        <v>0.30299999999999999</v>
+        <v>0.16</v>
       </c>
       <c r="H20" s="7">
         <f t="shared" si="0"/>
-        <v>0.30299999999999999</v>
+        <v>0.16</v>
       </c>
       <c r="I20" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>118</v>
       </c>
       <c r="B21" s="4">
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>59</v>
+        <v>119</v>
       </c>
       <c r="D21" t="s">
-        <v>37</v>
+        <v>120</v>
       </c>
       <c r="E21" t="s">
-        <v>38</v>
+        <v>121</v>
       </c>
       <c r="F21" t="s">
-        <v>87</v>
+        <v>127</v>
       </c>
       <c r="G21" s="6">
-        <v>8.0000000000000002E-3</v>
+        <v>0.30299999999999999</v>
       </c>
       <c r="H21" s="7">
         <f t="shared" si="0"/>
-        <v>8.0000000000000002E-3</v>
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="I21" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>117</v>
+        <v>36</v>
       </c>
       <c r="B22" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D22" t="s">
         <v>37</v>
@@ -1837,25 +1861,25 @@
         <v>38</v>
       </c>
       <c r="F22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G22" s="6">
-        <v>1.6E-2</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="H22" s="7">
         <f t="shared" si="0"/>
-        <v>3.2000000000000001E-2</v>
+        <v>8.0000000000000002E-3</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B23" s="4">
         <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D23" t="s">
         <v>37</v>
@@ -1864,25 +1888,25 @@
         <v>38</v>
       </c>
       <c r="F23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G23" s="6">
-        <v>1.2999999999999999E-2</v>
+        <v>1.6E-2</v>
       </c>
       <c r="H23" s="7">
         <f t="shared" si="0"/>
-        <v>2.5999999999999999E-2</v>
+        <v>3.2000000000000001E-2</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>116</v>
       </c>
       <c r="B24" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D24" t="s">
         <v>37</v>
@@ -1891,25 +1915,25 @@
         <v>38</v>
       </c>
       <c r="F24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G24" s="6">
-        <v>1.6E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="H24" s="7">
         <f t="shared" si="0"/>
-        <v>1.6E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B25" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D25" t="s">
         <v>37</v>
@@ -1918,25 +1942,25 @@
         <v>38</v>
       </c>
       <c r="F25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G25" s="6">
-        <v>9.9000000000000008E-3</v>
+        <v>1.6E-2</v>
       </c>
       <c r="H25" s="7">
         <f t="shared" si="0"/>
-        <v>3.9600000000000003E-2</v>
+        <v>1.6E-2</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>115</v>
+        <v>40</v>
       </c>
       <c r="B26" s="4">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D26" t="s">
         <v>37</v>
@@ -1945,25 +1969,25 @@
         <v>38</v>
       </c>
       <c r="F26" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G26" s="6">
-        <v>1.6E-2</v>
+        <v>9.9000000000000008E-3</v>
       </c>
       <c r="H26" s="7">
         <f t="shared" si="0"/>
-        <v>0.128</v>
+        <v>3.9600000000000003E-2</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B27" s="4">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D27" t="s">
         <v>37</v>
@@ -1972,159 +1996,213 @@
         <v>38</v>
       </c>
       <c r="F27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G27" s="6">
         <v>1.6E-2</v>
       </c>
       <c r="H27" s="7">
         <f t="shared" si="0"/>
-        <v>1.6E-2</v>
+        <v>0.128</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>41</v>
+        <v>114</v>
       </c>
       <c r="B28" s="4">
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="D28" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E28" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G28" s="6">
-        <v>1.2310000000000001</v>
+        <v>1.6E-2</v>
       </c>
       <c r="H28" s="7">
         <f t="shared" si="0"/>
-        <v>1.2310000000000001</v>
+        <v>1.6E-2</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B29" s="4">
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>111</v>
+        <v>42</v>
       </c>
       <c r="D29" t="s">
-        <v>113</v>
+        <v>43</v>
       </c>
       <c r="E29" t="s">
-        <v>112</v>
+        <v>44</v>
       </c>
       <c r="F29" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="G29" s="6">
-        <v>2.7559999999999998</v>
+        <v>1.2310000000000001</v>
       </c>
       <c r="H29" s="7">
         <f t="shared" si="0"/>
-        <v>2.7559999999999998</v>
+        <v>1.2310000000000001</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B30" s="4">
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>47</v>
+        <v>111</v>
       </c>
       <c r="D30" t="s">
-        <v>48</v>
+        <v>113</v>
       </c>
       <c r="E30" t="s">
-        <v>49</v>
+        <v>112</v>
+      </c>
+      <c r="F30" t="s">
+        <v>110</v>
       </c>
       <c r="G30" s="6">
-        <v>6.63</v>
+        <v>2.7559999999999998</v>
       </c>
       <c r="H30" s="7">
         <f t="shared" si="0"/>
-        <v>6.63</v>
-      </c>
-      <c r="I30" t="s">
-        <v>47</v>
+        <v>2.7559999999999998</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B31" s="4">
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D31" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E31" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="G31" s="6">
-        <v>7.29</v>
+        <v>6.63</v>
       </c>
       <c r="H31" s="7">
         <f t="shared" si="0"/>
-        <v>7.29</v>
+        <v>6.63</v>
       </c>
       <c r="I31" t="s">
-        <v>81</v>
+        <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B32" s="4">
         <v>1</v>
       </c>
       <c r="C32" t="s">
+        <v>51</v>
+      </c>
+      <c r="D32" t="s">
+        <v>52</v>
+      </c>
+      <c r="E32" t="s">
+        <v>68</v>
+      </c>
+      <c r="G32" s="6">
+        <v>7.29</v>
+      </c>
+      <c r="H32" s="7">
+        <f t="shared" si="0"/>
+        <v>7.29</v>
+      </c>
+      <c r="I32" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>134</v>
+      </c>
+      <c r="B33" s="4">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s">
+        <v>135</v>
+      </c>
+      <c r="D33" t="s">
+        <v>136</v>
+      </c>
+      <c r="E33" t="s">
+        <v>137</v>
+      </c>
+      <c r="F33" t="s">
+        <v>138</v>
+      </c>
+      <c r="G33" s="6">
+        <v>1.367</v>
+      </c>
+      <c r="H33" s="7">
+        <f t="shared" si="0"/>
+        <v>1.367</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>53</v>
+      </c>
+      <c r="B34" s="4">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
         <v>54</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D34" t="s">
         <v>55</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E34" t="s">
         <v>56</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F34" t="s">
         <v>71</v>
       </c>
-      <c r="G32" s="6">
+      <c r="G34" s="6">
         <v>0.25</v>
       </c>
-      <c r="H32" s="7">
+      <c r="H34" s="7">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
     </row>
-    <row r="34" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="G34" s="8">
-        <f>SUM(H5:H32)</f>
-        <v>29.385300000000001</v>
-      </c>
-    </row>
-    <row r="37" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C37" s="5"/>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G36" s="8">
+        <f>SUM(H5:H34)</f>
+        <v>30.9269</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C39" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Started changed base on Hardware 1 build
</commit_message>
<xml_diff>
--- a/Hardware/TalDoor_BOM.xlsx
+++ b/Hardware/TalDoor_BOM.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Spencer\Google Drive\Kuro\1 Documents\2 Projects\TalDoor\Hardware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Kuro\1 Documents\2 Projects\TalDoor\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4800" windowWidth="21600" windowHeight="11780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="6000" windowWidth="21600" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TalDoor" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="143">
   <si>
     <t>Component Count:</t>
   </si>
@@ -237,9 +237,6 @@
     <t xml:space="preserve">887-1820-ND </t>
   </si>
   <si>
-    <t>493-5907-1-ND</t>
-  </si>
-  <si>
     <t>399-6597-ND</t>
   </si>
   <si>
@@ -445,6 +442,12 @@
   </si>
   <si>
     <t>No EMI Fingers, but different pinout: ARJ11D-MDSD-A-B-FLT2-ND</t>
+  </si>
+  <si>
+    <t>1572-1665-ND</t>
+  </si>
+  <si>
+    <t>OLD taller one: 493-5907-1-ND</t>
   </si>
 </sst>
 </file>
@@ -590,7 +593,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -768,6 +771,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -940,7 +949,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -960,6 +969,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1318,34 +1330,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.6328125" customWidth="1"/>
-    <col min="5" max="5" width="43.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.26953125" customWidth="1"/>
-    <col min="9" max="9" width="48.7265625" customWidth="1"/>
+    <col min="1" max="1" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" customWidth="1"/>
+    <col min="5" max="5" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" customWidth="1"/>
+    <col min="9" max="9" width="48.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
@@ -1354,7 +1366,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
@@ -1374,18 +1386,18 @@
         <v>69</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="10">
         <v>1</v>
       </c>
       <c r="C5" t="s">
@@ -1398,7 +1410,7 @@
         <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G5" s="6">
         <v>1.375</v>
@@ -1408,11 +1420,11 @@
         <v>1.375</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="10">
         <v>9</v>
       </c>
       <c r="C6" t="s">
@@ -1425,7 +1437,7 @@
         <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G6" s="6">
         <v>1.06E-2</v>
@@ -1435,11 +1447,11 @@
         <v>9.5399999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="10">
         <v>2</v>
       </c>
       <c r="C7" t="s">
@@ -1452,7 +1464,7 @@
         <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G7" s="6">
         <v>1.1900000000000001E-2</v>
@@ -1462,11 +1474,11 @@
         <v>2.3800000000000002E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="10">
         <v>2</v>
       </c>
       <c r="C8" t="s">
@@ -1479,7 +1491,7 @@
         <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G8" s="6">
         <v>9.4E-2</v>
@@ -1489,11 +1501,11 @@
         <v>0.188</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="10">
         <v>1</v>
       </c>
       <c r="C9" t="s">
@@ -1506,7 +1518,7 @@
         <v>12</v>
       </c>
       <c r="F9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G9" s="6">
         <v>7.4999999999999997E-3</v>
@@ -1516,11 +1528,11 @@
         <v>7.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
@@ -1533,7 +1545,7 @@
         <v>18</v>
       </c>
       <c r="F10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G10" s="6">
         <v>0.105</v>
@@ -1543,11 +1555,11 @@
         <v>0.105</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="10">
         <v>1</v>
       </c>
       <c r="C11" t="s">
@@ -1560,25 +1572,28 @@
         <v>18</v>
       </c>
       <c r="F11" t="s">
-        <v>72</v>
+        <v>141</v>
       </c>
       <c r="G11" s="6">
-        <v>0.33200000000000002</v>
+        <v>0.28299999999999997</v>
       </c>
       <c r="H11" s="7">
         <f t="shared" si="0"/>
-        <v>0.33200000000000002</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+        <v>0.28299999999999997</v>
+      </c>
+      <c r="I11" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>130</v>
+      </c>
+      <c r="B12" s="10">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
         <v>131</v>
-      </c>
-      <c r="B12" s="4">
-        <v>3</v>
-      </c>
-      <c r="C12" t="s">
-        <v>132</v>
       </c>
       <c r="D12" t="s">
         <v>11</v>
@@ -1587,7 +1602,7 @@
         <v>12</v>
       </c>
       <c r="F12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G12" s="6">
         <v>5.8200000000000002E-2</v>
@@ -1597,11 +1612,11 @@
         <v>0.17460000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>124</v>
-      </c>
-      <c r="B13" s="4">
+        <v>123</v>
+      </c>
+      <c r="B13" s="10">
         <v>4</v>
       </c>
       <c r="C13" t="s">
@@ -1611,10 +1626,10 @@
         <v>27</v>
       </c>
       <c r="E13" t="s">
+        <v>76</v>
+      </c>
+      <c r="F13" t="s">
         <v>77</v>
-      </c>
-      <c r="F13" t="s">
-        <v>78</v>
       </c>
       <c r="G13" s="6">
         <v>0.33700000000000002</v>
@@ -1624,11 +1639,11 @@
         <v>1.3480000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>125</v>
-      </c>
-      <c r="B14" s="4">
+        <v>124</v>
+      </c>
+      <c r="B14" s="10">
         <v>4</v>
       </c>
       <c r="C14" t="s">
@@ -1638,10 +1653,10 @@
         <v>27</v>
       </c>
       <c r="E14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G14" s="6">
         <v>0.317</v>
@@ -1651,11 +1666,11 @@
         <v>1.268</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="10">
         <v>1</v>
       </c>
       <c r="C15" t="s">
@@ -1668,7 +1683,7 @@
         <v>66</v>
       </c>
       <c r="F15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G15" s="6">
         <v>5.1100000000000003</v>
@@ -1678,24 +1693,24 @@
         <v>5.1100000000000003</v>
       </c>
       <c r="I15" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B16" s="4">
         <v>1</v>
       </c>
       <c r="C16" t="s">
+        <v>98</v>
+      </c>
+      <c r="D16" t="s">
         <v>99</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>100</v>
-      </c>
-      <c r="E16" t="s">
-        <v>101</v>
       </c>
       <c r="G16" s="6">
         <v>0</v>
@@ -1705,27 +1720,27 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>101</v>
+      </c>
+      <c r="B17" s="10">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>102</v>
+      </c>
+      <c r="D17" t="s">
+        <v>103</v>
+      </c>
+      <c r="E17" t="s">
+        <v>104</v>
+      </c>
+      <c r="F17" t="s">
         <v>106</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>102</v>
-      </c>
-      <c r="B17" s="4">
-        <v>2</v>
-      </c>
-      <c r="C17" t="s">
-        <v>103</v>
-      </c>
-      <c r="D17" t="s">
-        <v>104</v>
-      </c>
-      <c r="E17" t="s">
-        <v>105</v>
-      </c>
-      <c r="F17" t="s">
-        <v>107</v>
       </c>
       <c r="G17" s="6">
         <v>0.36799999999999999</v>
@@ -1735,14 +1750,14 @@
         <v>0.73599999999999999</v>
       </c>
       <c r="I17" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="10">
         <v>1</v>
       </c>
       <c r="C18" t="s">
@@ -1755,7 +1770,7 @@
         <v>35</v>
       </c>
       <c r="F18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G18" s="6">
         <v>0.14099999999999999</v>
@@ -1765,18 +1780,18 @@
         <v>0.14099999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B19" s="4">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E19" t="s">
         <v>67</v>
@@ -1787,27 +1802,27 @@
         <v>0</v>
       </c>
       <c r="I19" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>121</v>
-      </c>
-      <c r="B20" s="4">
+        <v>120</v>
+      </c>
+      <c r="B20" s="10">
         <v>1</v>
       </c>
       <c r="C20" t="s">
+        <v>93</v>
+      </c>
+      <c r="D20" t="s">
         <v>94</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>95</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>96</v>
-      </c>
-      <c r="F20" t="s">
-        <v>97</v>
       </c>
       <c r="G20" s="6">
         <v>0.16</v>
@@ -1817,27 +1832,27 @@
         <v>0.16</v>
       </c>
       <c r="I20" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>116</v>
+      </c>
+      <c r="B21" s="10">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
         <v>117</v>
       </c>
-      <c r="B21" s="4">
-        <v>1</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>118</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>119</v>
       </c>
-      <c r="E21" t="s">
-        <v>120</v>
-      </c>
       <c r="F21" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G21" s="6">
         <v>0.30299999999999999</v>
@@ -1847,14 +1862,14 @@
         <v>0.30299999999999999</v>
       </c>
       <c r="I21" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B22" s="10">
         <v>1</v>
       </c>
       <c r="C22" t="s">
@@ -1867,7 +1882,7 @@
         <v>38</v>
       </c>
       <c r="F22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G22" s="6">
         <v>8.0000000000000002E-3</v>
@@ -1877,11 +1892,11 @@
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>116</v>
-      </c>
-      <c r="B23" s="4">
+        <v>115</v>
+      </c>
+      <c r="B23" s="10">
         <v>2</v>
       </c>
       <c r="C23" t="s">
@@ -1894,7 +1909,7 @@
         <v>38</v>
       </c>
       <c r="F23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G23" s="6">
         <v>1.6E-2</v>
@@ -1904,11 +1919,11 @@
         <v>3.2000000000000001E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>115</v>
-      </c>
-      <c r="B24" s="4">
+        <v>114</v>
+      </c>
+      <c r="B24" s="10">
         <v>2</v>
       </c>
       <c r="C24" t="s">
@@ -1921,7 +1936,7 @@
         <v>38</v>
       </c>
       <c r="F24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G24" s="6">
         <v>1.2999999999999999E-2</v>
@@ -1931,11 +1946,11 @@
         <v>2.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>39</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B25" s="10">
         <v>1</v>
       </c>
       <c r="C25" t="s">
@@ -1948,7 +1963,7 @@
         <v>38</v>
       </c>
       <c r="F25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G25" s="6">
         <v>1.6E-2</v>
@@ -1958,11 +1973,11 @@
         <v>1.6E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>40</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B26" s="10">
         <v>4</v>
       </c>
       <c r="C26" t="s">
@@ -1975,7 +1990,7 @@
         <v>38</v>
       </c>
       <c r="F26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G26" s="6">
         <v>9.9000000000000008E-3</v>
@@ -1985,11 +2000,11 @@
         <v>3.9600000000000003E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>114</v>
-      </c>
-      <c r="B27" s="4">
+        <v>113</v>
+      </c>
+      <c r="B27" s="10">
         <v>8</v>
       </c>
       <c r="C27" t="s">
@@ -2002,7 +2017,7 @@
         <v>38</v>
       </c>
       <c r="F27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G27" s="6">
         <v>1.6E-2</v>
@@ -2012,11 +2027,11 @@
         <v>0.128</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>113</v>
-      </c>
-      <c r="B28" s="4">
+        <v>112</v>
+      </c>
+      <c r="B28" s="10">
         <v>1</v>
       </c>
       <c r="C28" t="s">
@@ -2029,7 +2044,7 @@
         <v>38</v>
       </c>
       <c r="F28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G28" s="6">
         <v>1.6E-2</v>
@@ -2039,11 +2054,11 @@
         <v>1.6E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>41</v>
       </c>
-      <c r="B29" s="4">
+      <c r="B29" s="10">
         <v>1</v>
       </c>
       <c r="C29" t="s">
@@ -2056,7 +2071,7 @@
         <v>44</v>
       </c>
       <c r="F29" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G29" s="6">
         <v>1.2310000000000001</v>
@@ -2066,24 +2081,24 @@
         <v>1.2310000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>45</v>
       </c>
-      <c r="B30" s="4">
+      <c r="B30" s="10">
         <v>1</v>
       </c>
       <c r="C30" t="s">
+        <v>109</v>
+      </c>
+      <c r="D30" t="s">
+        <v>111</v>
+      </c>
+      <c r="E30" t="s">
         <v>110</v>
       </c>
-      <c r="D30" t="s">
-        <v>112</v>
-      </c>
-      <c r="E30" t="s">
-        <v>111</v>
-      </c>
       <c r="F30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G30" s="6">
         <v>2.7559999999999998</v>
@@ -2093,7 +2108,7 @@
         <v>2.7559999999999998</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>46</v>
       </c>
@@ -2120,7 +2135,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>50</v>
       </c>
@@ -2144,27 +2159,27 @@
         <v>7.29</v>
       </c>
       <c r="I32" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>132</v>
+      </c>
+      <c r="B33" s="10">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s">
         <v>133</v>
       </c>
-      <c r="B33" s="4">
-        <v>1</v>
-      </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>134</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>135</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
         <v>136</v>
-      </c>
-      <c r="F33" t="s">
-        <v>137</v>
       </c>
       <c r="G33" s="6">
         <v>1.367</v>
@@ -2174,11 +2189,11 @@
         <v>1.367</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>53</v>
       </c>
-      <c r="B34" s="4">
+      <c r="B34" s="10">
         <v>1</v>
       </c>
       <c r="C34" t="s">
@@ -2201,13 +2216,13 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G36" s="8">
         <f>SUM(H5:H34)</f>
-        <v>31.1569</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+        <v>31.107900000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C39" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating PCB layout, unfinished
</commit_message>
<xml_diff>
--- a/Hardware/TalDoor_BOM.xlsx
+++ b/Hardware/TalDoor_BOM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="6000" windowWidth="21600" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="6600" windowWidth="21600" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TalDoor" sheetId="1" r:id="rId1"/>
@@ -93,9 +93,6 @@
     <t xml:space="preserve">C15, </t>
   </si>
   <si>
-    <t>1000uF</t>
-  </si>
-  <si>
     <t>Capacitors_THT:CP_Radial_D10.0mm_P5.00mm</t>
   </si>
   <si>
@@ -444,10 +441,13 @@
     <t>No EMI Fingers, but different pinout: ARJ11D-MDSD-A-B-FLT2-ND</t>
   </si>
   <si>
-    <t>1572-1665-ND</t>
-  </si>
-  <si>
     <t>OLD taller one: 493-5907-1-ND</t>
+  </si>
+  <si>
+    <t>470uF</t>
+  </si>
+  <si>
+    <t>493-11709-1-ND</t>
   </si>
 </sst>
 </file>
@@ -1348,12 +1348,12 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B2" s="1"/>
     </row>
@@ -1371,7 +1371,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>2</v>
@@ -1383,14 +1383,14 @@
         <v>4</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1410,7 +1410,7 @@
         <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G5" s="6">
         <v>1.375</v>
@@ -1437,7 +1437,7 @@
         <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G6" s="6">
         <v>1.06E-2</v>
@@ -1464,7 +1464,7 @@
         <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G7" s="6">
         <v>1.1900000000000001E-2</v>
@@ -1491,7 +1491,7 @@
         <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G8" s="6">
         <v>9.4E-2</v>
@@ -1518,7 +1518,7 @@
         <v>12</v>
       </c>
       <c r="F9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G9" s="6">
         <v>7.4999999999999997E-3</v>
@@ -1545,7 +1545,7 @@
         <v>18</v>
       </c>
       <c r="F10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G10" s="6">
         <v>0.105</v>
@@ -1563,37 +1563,37 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
+        <v>141</v>
+      </c>
+      <c r="D11" t="s">
         <v>24</v>
-      </c>
-      <c r="D11" t="s">
-        <v>25</v>
       </c>
       <c r="E11" t="s">
         <v>18</v>
       </c>
       <c r="F11" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G11" s="6">
-        <v>0.28299999999999997</v>
+        <v>0.311</v>
       </c>
       <c r="H11" s="7">
         <f t="shared" si="0"/>
-        <v>0.28299999999999997</v>
+        <v>0.311</v>
       </c>
       <c r="I11" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B12" s="10">
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D12" t="s">
         <v>11</v>
@@ -1602,7 +1602,7 @@
         <v>12</v>
       </c>
       <c r="F12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G12" s="6">
         <v>5.8200000000000002E-2</v>
@@ -1614,22 +1614,22 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B13" s="10">
         <v>4</v>
       </c>
       <c r="C13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" t="s">
         <v>26</v>
       </c>
-      <c r="D13" t="s">
-        <v>27</v>
-      </c>
       <c r="E13" t="s">
+        <v>75</v>
+      </c>
+      <c r="F13" t="s">
         <v>76</v>
-      </c>
-      <c r="F13" t="s">
-        <v>77</v>
       </c>
       <c r="G13" s="6">
         <v>0.33700000000000002</v>
@@ -1641,22 +1641,22 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B14" s="10">
         <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G14" s="6">
         <v>0.317</v>
@@ -1668,22 +1668,22 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" s="10">
         <v>1</v>
       </c>
       <c r="C15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" t="s">
         <v>30</v>
       </c>
-      <c r="D15" t="s">
-        <v>31</v>
-      </c>
       <c r="E15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G15" s="6">
         <v>5.1100000000000003</v>
@@ -1693,24 +1693,24 @@
         <v>5.1100000000000003</v>
       </c>
       <c r="I15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B16" s="4">
         <v>1</v>
       </c>
       <c r="C16" t="s">
+        <v>97</v>
+      </c>
+      <c r="D16" t="s">
         <v>98</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>99</v>
-      </c>
-      <c r="E16" t="s">
-        <v>100</v>
       </c>
       <c r="G16" s="6">
         <v>0</v>
@@ -1720,27 +1720,27 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B17" s="10">
         <v>2</v>
       </c>
       <c r="C17" t="s">
+        <v>101</v>
+      </c>
+      <c r="D17" t="s">
         <v>102</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>103</v>
       </c>
-      <c r="E17" t="s">
-        <v>104</v>
-      </c>
       <c r="F17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G17" s="6">
         <v>0.36799999999999999</v>
@@ -1750,27 +1750,27 @@
         <v>0.73599999999999999</v>
       </c>
       <c r="I17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18" s="10">
         <v>1</v>
       </c>
       <c r="C18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" t="s">
         <v>33</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>34</v>
       </c>
-      <c r="E18" t="s">
-        <v>35</v>
-      </c>
       <c r="F18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G18" s="6">
         <v>0.14099999999999999</v>
@@ -1782,19 +1782,19 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B19" s="4">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G19" s="6"/>
       <c r="H19" s="7">
@@ -1802,27 +1802,27 @@
         <v>0</v>
       </c>
       <c r="I19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B20" s="10">
         <v>1</v>
       </c>
       <c r="C20" t="s">
+        <v>92</v>
+      </c>
+      <c r="D20" t="s">
         <v>93</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>94</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>95</v>
-      </c>
-      <c r="F20" t="s">
-        <v>96</v>
       </c>
       <c r="G20" s="6">
         <v>0.16</v>
@@ -1832,27 +1832,27 @@
         <v>0.16</v>
       </c>
       <c r="I20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B21" s="10">
         <v>1</v>
       </c>
       <c r="C21" t="s">
+        <v>116</v>
+      </c>
+      <c r="D21" t="s">
         <v>117</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>118</v>
       </c>
-      <c r="E21" t="s">
-        <v>119</v>
-      </c>
       <c r="F21" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G21" s="6">
         <v>0.30299999999999999</v>
@@ -1862,27 +1862,27 @@
         <v>0.30299999999999999</v>
       </c>
       <c r="I21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B22" s="10">
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D22" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22" t="s">
         <v>37</v>
       </c>
-      <c r="E22" t="s">
-        <v>38</v>
-      </c>
       <c r="F22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G22" s="6">
         <v>8.0000000000000002E-3</v>
@@ -1894,22 +1894,22 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B23" s="10">
         <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D23" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23" t="s">
         <v>37</v>
       </c>
-      <c r="E23" t="s">
-        <v>38</v>
-      </c>
       <c r="F23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G23" s="6">
         <v>1.6E-2</v>
@@ -1921,22 +1921,22 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B24" s="10">
         <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D24" t="s">
+        <v>36</v>
+      </c>
+      <c r="E24" t="s">
         <v>37</v>
       </c>
-      <c r="E24" t="s">
-        <v>38</v>
-      </c>
       <c r="F24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G24" s="6">
         <v>1.2999999999999999E-2</v>
@@ -1948,22 +1948,22 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B25" s="10">
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D25" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" t="s">
         <v>37</v>
       </c>
-      <c r="E25" t="s">
-        <v>38</v>
-      </c>
       <c r="F25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G25" s="6">
         <v>1.6E-2</v>
@@ -1975,22 +1975,22 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B26" s="10">
         <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D26" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" t="s">
         <v>37</v>
       </c>
-      <c r="E26" t="s">
-        <v>38</v>
-      </c>
       <c r="F26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G26" s="6">
         <v>9.9000000000000008E-3</v>
@@ -2002,22 +2002,22 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B27" s="10">
         <v>8</v>
       </c>
       <c r="C27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D27" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" t="s">
         <v>37</v>
       </c>
-      <c r="E27" t="s">
-        <v>38</v>
-      </c>
       <c r="F27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G27" s="6">
         <v>1.6E-2</v>
@@ -2029,22 +2029,22 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B28" s="10">
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D28" t="s">
+        <v>36</v>
+      </c>
+      <c r="E28" t="s">
         <v>37</v>
       </c>
-      <c r="E28" t="s">
-        <v>38</v>
-      </c>
       <c r="F28" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G28" s="6">
         <v>1.6E-2</v>
@@ -2056,22 +2056,22 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B29" s="10">
         <v>1</v>
       </c>
       <c r="C29" t="s">
+        <v>41</v>
+      </c>
+      <c r="D29" t="s">
         <v>42</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>43</v>
       </c>
-      <c r="E29" t="s">
-        <v>44</v>
-      </c>
       <c r="F29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G29" s="6">
         <v>1.2310000000000001</v>
@@ -2083,22 +2083,22 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B30" s="10">
         <v>1</v>
       </c>
       <c r="C30" t="s">
+        <v>108</v>
+      </c>
+      <c r="D30" t="s">
+        <v>110</v>
+      </c>
+      <c r="E30" t="s">
         <v>109</v>
       </c>
-      <c r="D30" t="s">
-        <v>111</v>
-      </c>
-      <c r="E30" t="s">
-        <v>110</v>
-      </c>
       <c r="F30" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G30" s="6">
         <v>2.7559999999999998</v>
@@ -2110,19 +2110,19 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B31" s="4">
         <v>1</v>
       </c>
       <c r="C31" t="s">
+        <v>46</v>
+      </c>
+      <c r="D31" t="s">
         <v>47</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>48</v>
-      </c>
-      <c r="E31" t="s">
-        <v>49</v>
       </c>
       <c r="G31" s="6">
         <v>6.63</v>
@@ -2132,24 +2132,24 @@
         <v>6.63</v>
       </c>
       <c r="I31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B32" s="4">
         <v>1</v>
       </c>
       <c r="C32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32" t="s">
         <v>51</v>
       </c>
-      <c r="D32" t="s">
-        <v>52</v>
-      </c>
       <c r="E32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G32" s="6">
         <v>7.29</v>
@@ -2159,27 +2159,27 @@
         <v>7.29</v>
       </c>
       <c r="I32" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B33" s="10">
         <v>1</v>
       </c>
       <c r="C33" t="s">
+        <v>132</v>
+      </c>
+      <c r="D33" t="s">
         <v>133</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>134</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
         <v>135</v>
-      </c>
-      <c r="F33" t="s">
-        <v>136</v>
       </c>
       <c r="G33" s="6">
         <v>1.367</v>
@@ -2191,22 +2191,22 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B34" s="10">
         <v>1</v>
       </c>
       <c r="C34" t="s">
+        <v>53</v>
+      </c>
+      <c r="D34" t="s">
         <v>54</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>55</v>
       </c>
-      <c r="E34" t="s">
-        <v>56</v>
-      </c>
       <c r="F34" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G34" s="6">
         <v>0.25</v>
@@ -2219,7 +2219,7 @@
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G36" s="8">
         <f>SUM(H5:H34)</f>
-        <v>31.107900000000001</v>
+        <v>31.135899999999999</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated schematic rev & date, bom
</commit_message>
<xml_diff>
--- a/Hardware/TalDoor_BOM.xlsx
+++ b/Hardware/TalDoor_BOM.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Kuro\1 Documents\2 Projects\TalDoor\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E23C5DA6-57C9-4A6A-84EA-1C63EEECBD65}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="8400" windowWidth="21600" windowHeight="11775" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="9000" windowWidth="21600" windowHeight="11775" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TalDoor" sheetId="1" r:id="rId1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="153">
   <si>
     <t>Component Count:</t>
   </si>
@@ -461,6 +462,24 @@
   </si>
   <si>
     <t>Ag9705-2BR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JP2, JP1, JP4, JP5, JP6, JP3, </t>
+  </si>
+  <si>
+    <t>Jumper_NC_Dual</t>
+  </si>
+  <si>
+    <t>Connectors:GS3</t>
+  </si>
+  <si>
+    <t>Dual Jumper, normally closed</t>
+  </si>
+  <si>
+    <t>DNP</t>
+  </si>
+  <si>
+    <t>Generated: 3/9/2018  11:51:53 AM</t>
   </si>
 </sst>
 </file>
@@ -975,7 +994,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1007,6 +1026,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -2298,7 +2320,7 @@
   <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2322,10 +2344,10 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>129</v>
+        <v>152</v>
       </c>
       <c r="B2" s="11">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2334,7 +2356,7 @@
       </c>
       <c r="B3" s="14">
         <f>SUM(B5:B47)</f>
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2370,7 +2392,7 @@
       <c r="A5" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="16">
         <v>1</v>
       </c>
       <c r="C5" s="14" t="s">
@@ -2397,7 +2419,7 @@
       <c r="A6" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="16">
         <v>9</v>
       </c>
       <c r="C6" s="14" t="s">
@@ -2424,7 +2446,7 @@
       <c r="A7" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="16">
         <v>2</v>
       </c>
       <c r="C7" s="14" t="s">
@@ -2451,7 +2473,7 @@
       <c r="A8" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="16">
         <v>3</v>
       </c>
       <c r="C8" s="14" t="s">
@@ -2478,7 +2500,7 @@
       <c r="A9" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="16">
         <v>1</v>
       </c>
       <c r="C9" s="14" t="s">
@@ -2505,7 +2527,7 @@
       <c r="A10" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="16">
         <v>1</v>
       </c>
       <c r="C10" s="14" t="s">
@@ -2532,7 +2554,7 @@
       <c r="A11" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="16">
         <v>1</v>
       </c>
       <c r="C11" s="14" t="s">
@@ -2560,172 +2582,165 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="B12" s="8">
-        <v>3</v>
+        <v>114</v>
+      </c>
+      <c r="B12" s="16">
+        <v>4</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>121</v>
+        <v>24</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>12</v>
+        <v>73</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>123</v>
+        <v>74</v>
       </c>
       <c r="G12" s="15">
-        <v>5.8200000000000002E-2</v>
+        <v>0.33700000000000002</v>
       </c>
       <c r="H12" s="6">
         <f t="shared" si="0"/>
-        <v>0.17460000000000001</v>
+        <v>1.3480000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="B13" s="8">
+        <v>115</v>
+      </c>
+      <c r="B13" s="16">
         <v>4</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>25</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G13" s="15">
-        <v>0.33700000000000002</v>
+        <v>0.317</v>
       </c>
       <c r="H13" s="6">
         <f t="shared" si="0"/>
-        <v>1.3480000000000001</v>
+        <v>1.268</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="B14" s="8">
-        <v>4</v>
+        <v>27</v>
+      </c>
+      <c r="B14" s="16">
+        <v>1</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>75</v>
+        <v>124</v>
       </c>
       <c r="G14" s="15">
-        <v>0.317</v>
+        <v>5.1100000000000003</v>
       </c>
       <c r="H14" s="6">
         <f t="shared" si="0"/>
-        <v>1.268</v>
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="I14" s="14" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="8">
-        <v>1</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>28</v>
+        <v>92</v>
+      </c>
+      <c r="B15" s="16">
+        <v>1</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>136</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>29</v>
+        <v>137</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="G15" s="15">
-        <v>5.1100000000000003</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="G15" s="15"/>
       <c r="H15" s="6">
         <f t="shared" si="0"/>
-        <v>5.1100000000000003</v>
-      </c>
-      <c r="I15" s="14" t="s">
-        <v>125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="B16" s="3">
-        <v>1</v>
+        <v>93</v>
+      </c>
+      <c r="B16" s="16">
+        <v>2</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>136</v>
+        <v>94</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>137</v>
+        <v>95</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="G16" s="15"/>
+        <v>96</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="G16" s="15">
+        <v>0.36799999999999999</v>
+      </c>
       <c r="H16" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.73599999999999999</v>
+      </c>
+      <c r="I16" s="14" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="B17" s="8">
-        <v>2</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>94</v>
+        <v>147</v>
+      </c>
+      <c r="B17" s="16">
+        <v>6</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>148</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>95</v>
+        <v>149</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="G17" s="15">
-        <v>0.36799999999999999</v>
-      </c>
-      <c r="H17" s="6">
-        <f t="shared" si="0"/>
-        <v>0.73599999999999999</v>
+        <v>150</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>98</v>
+        <v>151</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18" s="16">
         <v>1</v>
       </c>
       <c r="C18" s="14" t="s">
@@ -2752,7 +2767,7 @@
       <c r="A19" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="16">
         <v>1</v>
       </c>
       <c r="C19" s="14" t="s">
@@ -2777,7 +2792,7 @@
       <c r="A20" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="B20" s="8">
+      <c r="B20" s="16">
         <v>1</v>
       </c>
       <c r="C20" s="14" t="s">
@@ -2807,7 +2822,7 @@
       <c r="A21" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="B21" s="8">
+      <c r="B21" s="16">
         <v>1</v>
       </c>
       <c r="C21" s="14" t="s">
@@ -2837,7 +2852,7 @@
       <c r="A22" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="8">
+      <c r="B22" s="16">
         <v>1</v>
       </c>
       <c r="C22" s="14" t="s">
@@ -2864,7 +2879,7 @@
       <c r="A23" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="B23" s="8">
+      <c r="B23" s="16">
         <v>2</v>
       </c>
       <c r="C23" s="14" t="s">
@@ -2891,7 +2906,7 @@
       <c r="A24" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="B24" s="8">
+      <c r="B24" s="16">
         <v>2</v>
       </c>
       <c r="C24" s="14" t="s">
@@ -2918,7 +2933,7 @@
       <c r="A25" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="8">
+      <c r="B25" s="16">
         <v>1</v>
       </c>
       <c r="C25" s="14" t="s">
@@ -2945,7 +2960,7 @@
       <c r="A26" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="8">
+      <c r="B26" s="16">
         <v>4</v>
       </c>
       <c r="C26" s="14" t="s">
@@ -2972,7 +2987,7 @@
       <c r="A27" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="B27" s="8">
+      <c r="B27" s="16">
         <v>8</v>
       </c>
       <c r="C27" s="14" t="s">
@@ -2999,7 +3014,7 @@
       <c r="A28" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="B28" s="8">
+      <c r="B28" s="16">
         <v>1</v>
       </c>
       <c r="C28" s="14" t="s">
@@ -3026,7 +3041,7 @@
       <c r="A29" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B29" s="8">
+      <c r="B29" s="16">
         <v>1</v>
       </c>
       <c r="C29" s="14" t="s">
@@ -3053,7 +3068,7 @@
       <c r="A30" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B30" s="8">
+      <c r="B30" s="16">
         <v>1</v>
       </c>
       <c r="C30" s="14" t="s">
@@ -3080,7 +3095,7 @@
       <c r="A31" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B31" s="16">
         <v>1</v>
       </c>
       <c r="C31" s="14" t="s">
@@ -3107,7 +3122,7 @@
       <c r="A32" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B32" s="16">
         <v>1</v>
       </c>
       <c r="C32" s="14" t="s">
@@ -3134,7 +3149,7 @@
       <c r="A33" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="B33" s="8">
+      <c r="B33" s="16">
         <v>1</v>
       </c>
       <c r="C33" s="15" t="s">
@@ -3161,7 +3176,7 @@
       <c r="A34" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="B34" s="8">
+      <c r="B34" s="16">
         <v>1</v>
       </c>
       <c r="C34" s="14" t="s">
@@ -3187,7 +3202,7 @@
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G36" s="10">
         <f>SUM(H5:H34)</f>
-        <v>30.535900000000002</v>
+        <v>30.3613</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fixed ethernet module, SPI, I2c busses
</commit_message>
<xml_diff>
--- a/Hardware/TalDoor_BOM.xlsx
+++ b/Hardware/TalDoor_BOM.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Kuro\1 Documents\2 Projects\TalDoor\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63BE26F2-6F39-4E58-A975-60148C1FCE08}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6905EC3-221A-47A4-B767-420D2974E5B5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="9600" windowWidth="21600" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="10200" windowWidth="21600" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TalDoor" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="140">
   <si>
     <t>Component Count:</t>
   </si>
@@ -208,9 +208,6 @@
     <t>68Ω</t>
   </si>
   <si>
-    <t>150Ω</t>
-  </si>
-  <si>
     <t>TH RJ45 with transformer + leds</t>
   </si>
   <si>
@@ -274,9 +271,6 @@
     <t>CR0603-JW-680ELFCT-ND</t>
   </si>
   <si>
-    <t>CR0603-JW-151ELFCT-ND</t>
-  </si>
-  <si>
     <t>296-34806-1-ND</t>
   </si>
   <si>
@@ -439,22 +433,13 @@
     <t>Ag9705-2BR</t>
   </si>
   <si>
-    <t xml:space="preserve">JP2, JP1, JP4, JP5, JP6, JP3, </t>
-  </si>
-  <si>
-    <t>Jumper_NC_Dual</t>
-  </si>
-  <si>
-    <t>Connectors:GS3</t>
-  </si>
-  <si>
-    <t>Dual Jumper, normally closed</t>
-  </si>
-  <si>
-    <t>DNP</t>
-  </si>
-  <si>
     <t>Generated: 3/9/2018  11:51:53 AM</t>
+  </si>
+  <si>
+    <t>120Ω</t>
+  </si>
+  <si>
+    <t>CR0603-JW-121ELFCT-ND</t>
   </si>
 </sst>
 </file>
@@ -1356,10 +1341,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A34"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1383,7 +1368,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B2" s="8">
         <v>65</v>
@@ -1394,8 +1379,8 @@
         <v>0</v>
       </c>
       <c r="B3" s="9">
-        <f>SUM(B5:B47)</f>
-        <v>65</v>
+        <f>SUM(B5:B46)</f>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1415,16 +1400,16 @@
         <v>4</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1444,7 +1429,7 @@
         <v>8</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G5" s="10">
         <v>1.375</v>
@@ -1471,13 +1456,13 @@
         <v>12</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G6" s="10">
         <v>1.06E-2</v>
       </c>
       <c r="H6" s="4">
-        <f t="shared" ref="H6:H34" si="0">G6*B6</f>
+        <f t="shared" ref="H6:H33" si="0">G6*B6</f>
         <v>9.5399999999999999E-2</v>
       </c>
     </row>
@@ -1498,7 +1483,7 @@
         <v>12</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G7" s="10">
         <v>1.1900000000000001E-2</v>
@@ -1510,7 +1495,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B8" s="11">
         <v>3</v>
@@ -1525,7 +1510,7 @@
         <v>12</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G8" s="10">
         <v>9.4E-2</v>
@@ -1552,7 +1537,7 @@
         <v>12</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G9" s="10">
         <v>7.4999999999999997E-3</v>
@@ -1579,7 +1564,7 @@
         <v>18</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G10" s="10">
         <v>0.105</v>
@@ -1597,7 +1582,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>23</v>
@@ -1606,7 +1591,7 @@
         <v>18</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G11" s="10">
         <v>0.311</v>
@@ -1616,12 +1601,12 @@
         <v>0.311</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B12" s="11">
         <v>4</v>
@@ -1633,10 +1618,10 @@
         <v>25</v>
       </c>
       <c r="E12" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="F12" s="9" t="s">
         <v>71</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>72</v>
       </c>
       <c r="G12" s="10">
         <v>0.33700000000000002</v>
@@ -1648,7 +1633,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B13" s="11">
         <v>4</v>
@@ -1660,10 +1645,10 @@
         <v>25</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G13" s="10">
         <v>0.317</v>
@@ -1687,10 +1672,10 @@
         <v>29</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G14" s="10">
         <v>5.1100000000000003</v>
@@ -1700,24 +1685,24 @@
         <v>5.1100000000000003</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B15" s="11">
         <v>1</v>
       </c>
       <c r="C15" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="E15" s="9" t="s">
         <v>128</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>130</v>
       </c>
       <c r="G15" s="10"/>
       <c r="H15" s="4">
@@ -1727,22 +1712,22 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B16" s="11">
         <v>2</v>
       </c>
       <c r="C16" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E16" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="F16" s="9" t="s">
         <v>93</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>95</v>
       </c>
       <c r="G16" s="10">
         <v>0.36799999999999999</v>
@@ -1752,150 +1737,157 @@
         <v>0.73599999999999999</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>139</v>
+        <v>30</v>
       </c>
       <c r="B17" s="11">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>140</v>
+        <v>31</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>141</v>
+        <v>32</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="I17" s="9" t="s">
-        <v>143</v>
+        <v>33</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="G17" s="10">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="H17" s="4">
+        <f t="shared" si="0"/>
+        <v>0.14099999999999999</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>30</v>
+        <v>113</v>
       </c>
       <c r="B18" s="11">
         <v>1</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>31</v>
+        <v>114</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>32</v>
+        <v>115</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="G18" s="10">
-        <v>0.14099999999999999</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="G18" s="10"/>
       <c r="H18" s="4">
         <f t="shared" si="0"/>
-        <v>0.14099999999999999</v>
+        <v>0</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="B19" s="11">
         <v>1</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>116</v>
+        <v>84</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>117</v>
+        <v>85</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="G19" s="10"/>
+        <v>86</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="G19" s="10">
+        <v>0.16</v>
+      </c>
       <c r="H19" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I19" s="6" t="s">
-        <v>134</v>
+        <v>0.16</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B20" s="11">
         <v>1</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>86</v>
+        <v>104</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>89</v>
+        <v>112</v>
       </c>
       <c r="G20" s="10">
-        <v>0.16</v>
+        <v>0.30299999999999999</v>
       </c>
       <c r="H20" s="4">
         <f t="shared" si="0"/>
-        <v>0.16</v>
+        <v>0.30299999999999999</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>105</v>
+        <v>34</v>
       </c>
       <c r="B21" s="11">
         <v>1</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>106</v>
+        <v>56</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>107</v>
+        <v>35</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>108</v>
+        <v>36</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>114</v>
+        <v>77</v>
       </c>
       <c r="G21" s="10">
-        <v>0.30299999999999999</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="H21" s="4">
         <f t="shared" si="0"/>
-        <v>0.30299999999999999</v>
-      </c>
-      <c r="I21" s="9" t="s">
-        <v>110</v>
+        <v>8.0000000000000002E-3</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>34</v>
+        <v>102</v>
       </c>
       <c r="B22" s="11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D22" s="9" t="s">
         <v>35</v>
@@ -1907,22 +1899,22 @@
         <v>78</v>
       </c>
       <c r="G22" s="10">
-        <v>8.0000000000000002E-3</v>
+        <v>1.6E-2</v>
       </c>
       <c r="H22" s="4">
         <f t="shared" si="0"/>
-        <v>8.0000000000000002E-3</v>
+        <v>3.2000000000000001E-2</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B23" s="11">
         <v>2</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>35</v>
@@ -1934,22 +1926,22 @@
         <v>79</v>
       </c>
       <c r="G23" s="10">
-        <v>1.6E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="H23" s="4">
         <f t="shared" si="0"/>
-        <v>3.2000000000000001E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
-        <v>103</v>
+        <v>37</v>
       </c>
       <c r="B24" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D24" s="9" t="s">
         <v>35</v>
@@ -1961,22 +1953,22 @@
         <v>80</v>
       </c>
       <c r="G24" s="10">
-        <v>1.2999999999999999E-2</v>
+        <v>1.6E-2</v>
       </c>
       <c r="H24" s="4">
         <f t="shared" si="0"/>
-        <v>2.5999999999999999E-2</v>
+        <v>1.6E-2</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B25" s="11">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>35</v>
@@ -1988,22 +1980,22 @@
         <v>81</v>
       </c>
       <c r="G25" s="10">
-        <v>1.6E-2</v>
+        <v>9.9000000000000008E-3</v>
       </c>
       <c r="H25" s="4">
         <f t="shared" si="0"/>
-        <v>1.6E-2</v>
+        <v>3.9600000000000003E-2</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>38</v>
+        <v>100</v>
       </c>
       <c r="B26" s="11">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D26" s="9" t="s">
         <v>35</v>
@@ -2015,22 +2007,22 @@
         <v>82</v>
       </c>
       <c r="G26" s="10">
-        <v>9.9000000000000008E-3</v>
+        <v>1.6E-2</v>
       </c>
       <c r="H26" s="4">
         <f t="shared" si="0"/>
-        <v>3.9600000000000003E-2</v>
+        <v>0.128</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B27" s="11">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>61</v>
+        <v>138</v>
       </c>
       <c r="D27" s="9" t="s">
         <v>35</v>
@@ -2039,213 +2031,186 @@
         <v>36</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>83</v>
+        <v>139</v>
       </c>
       <c r="G27" s="10">
         <v>1.6E-2</v>
       </c>
       <c r="H27" s="4">
         <f t="shared" si="0"/>
-        <v>0.128</v>
+        <v>1.6E-2</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
-        <v>101</v>
+        <v>39</v>
       </c>
       <c r="B28" s="11">
         <v>1</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G28" s="10">
-        <v>1.6E-2</v>
+        <v>1.2310000000000001</v>
       </c>
       <c r="H28" s="4">
         <f t="shared" si="0"/>
-        <v>1.6E-2</v>
+        <v>1.2310000000000001</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B29" s="11">
         <v>1</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>40</v>
+        <v>96</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>41</v>
+        <v>98</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>42</v>
+        <v>97</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="G29" s="10">
-        <v>1.2310000000000001</v>
+        <v>2.7559999999999998</v>
       </c>
       <c r="H29" s="4">
         <f t="shared" si="0"/>
-        <v>1.2310000000000001</v>
+        <v>2.7559999999999998</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B30" s="11">
         <v>1</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>98</v>
+        <v>45</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>100</v>
+        <v>46</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="F30" s="9" t="s">
-        <v>97</v>
+        <v>47</v>
       </c>
       <c r="G30" s="10">
-        <v>2.7559999999999998</v>
+        <v>6.63</v>
       </c>
       <c r="H30" s="4">
         <f t="shared" si="0"/>
-        <v>2.7559999999999998</v>
+        <v>6.63</v>
+      </c>
+      <c r="I30" s="9" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B31" s="11">
         <v>1</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>45</v>
+        <v>135</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="G31" s="10">
-        <v>6.63</v>
+        <v>7.29</v>
       </c>
       <c r="H31" s="4">
         <f t="shared" si="0"/>
-        <v>6.63</v>
+        <v>7.29</v>
       </c>
       <c r="I31" s="9" t="s">
-        <v>45</v>
+        <v>136</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
-        <v>48</v>
+        <v>116</v>
       </c>
       <c r="B32" s="11">
         <v>1</v>
       </c>
-      <c r="C32" s="9" t="s">
-        <v>137</v>
+      <c r="C32" s="10" t="s">
+        <v>122</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>49</v>
+        <v>123</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>65</v>
+        <v>124</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>125</v>
       </c>
       <c r="G32" s="10">
-        <v>7.29</v>
+        <v>0.60299999999999998</v>
       </c>
       <c r="H32" s="4">
         <f t="shared" si="0"/>
-        <v>7.29</v>
-      </c>
-      <c r="I32" s="9" t="s">
-        <v>138</v>
+        <v>0.60299999999999998</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
-        <v>118</v>
+        <v>50</v>
       </c>
       <c r="B33" s="11">
         <v>1</v>
       </c>
-      <c r="C33" s="10" t="s">
-        <v>124</v>
+      <c r="C33" s="9" t="s">
+        <v>51</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>125</v>
+        <v>52</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>126</v>
+        <v>53</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="G33" s="10">
-        <v>0.60299999999999998</v>
+        <v>0.32</v>
       </c>
       <c r="H33" s="4">
         <f t="shared" si="0"/>
-        <v>0.60299999999999998</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="B34" s="11">
-        <v>1</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="E34" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="F34" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="G34" s="10">
         <v>0.32</v>
       </c>
-      <c r="H34" s="4">
-        <f t="shared" si="0"/>
-        <v>0.32</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G36" s="7">
-        <f>SUM(H5:H34)</f>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G35" s="7">
+        <f>SUM(H5:H33)</f>
         <v>30.3613</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C39" s="3"/>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C38" s="3"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3">

</xml_diff>